<commit_message>
Work on filtering indels
</commit_message>
<xml_diff>
--- a/pf3k_techbm/scripts/gatk_pipeline/pipeline_parameters.xlsx
+++ b/pf3k_techbm/scripts/gatk_pipeline/pipeline_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pipeline_parameters.csv" sheetId="1" r:id="rId1"/>
@@ -81,51 +81,27 @@
     <t>SnpEff_region</t>
   </si>
   <si>
-    <t>"-an QD -an MQ -an MQRankSum -an ReadPosRankSum -an FS -an SOR -an DP"</t>
-  </si>
-  <si>
-    <t>"-an QD -an DP -an FS -an SOR -an ReadPosRankSum -an MQRankSum"</t>
-  </si>
-  <si>
     <t>crosses</t>
   </si>
   <si>
     <t>no_QD_indel</t>
   </si>
   <si>
-    <t>"-an DP -an FS -an SOR -an ReadPosRankSum -an MQRankSum"</t>
-  </si>
-  <si>
     <t>no_DP_indel</t>
   </si>
   <si>
-    <t>"-an QD -an FS -an SOR -an ReadPosRankSum -an MQRankSum"</t>
-  </si>
-  <si>
     <t>no_FS_indel</t>
   </si>
   <si>
-    <t>"-an QD -an DP -an SOR -an ReadPosRankSum -an MQRankSum"</t>
-  </si>
-  <si>
     <t>no_SOR_indel</t>
   </si>
   <si>
-    <t>"-an QD -an DP -an FS -an ReadPosRankSum -an MQRankSum"</t>
-  </si>
-  <si>
     <t>no_ReadPosRankSum_indel</t>
   </si>
   <si>
-    <t>"-an QD -an DP -an FS -an SOR -an MQRankSum"</t>
-  </si>
-  <si>
     <t>no_MQRankSum_indel</t>
   </si>
   <si>
-    <t>"-an QD -an DP -an FS -an SOR -an ReadPosRankSum"</t>
-  </si>
-  <si>
     <t>max_gauss_indel_5</t>
   </si>
   <si>
@@ -160,6 +136,30 @@
   </si>
   <si>
     <t>cortex</t>
+  </si>
+  <si>
+    <t>-an QD -an MQ -an MQRankSum -an ReadPosRankSum -an FS -an SOR -an DP</t>
+  </si>
+  <si>
+    <t>-an QD -an DP -an FS -an SOR -an ReadPosRankSum -an MQRankSum</t>
+  </si>
+  <si>
+    <t>-an DP -an FS -an SOR -an ReadPosRankSum -an MQRankSum</t>
+  </si>
+  <si>
+    <t>-an QD -an FS -an SOR -an ReadPosRankSum -an MQRankSum</t>
+  </si>
+  <si>
+    <t>-an QD -an DP -an SOR -an ReadPosRankSum -an MQRankSum</t>
+  </si>
+  <si>
+    <t>-an QD -an DP -an FS -an ReadPosRankSum -an MQRankSum</t>
+  </si>
+  <si>
+    <t>-an QD -an DP -an FS -an SOR -an MQRankSum</t>
+  </si>
+  <si>
+    <t>-an QD -an DP -an FS -an SOR -an ReadPosRankSum</t>
   </si>
 </sst>
 </file>
@@ -208,21 +208,78 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,11 +611,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -623,20 +695,20 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
       </c>
       <c r="L2">
         <v>15</v>
@@ -644,7 +716,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -656,25 +728,25 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
       </c>
       <c r="L3">
         <v>15</v>
@@ -682,7 +754,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -694,25 +766,25 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
       </c>
       <c r="L4">
         <v>15</v>
@@ -720,7 +792,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -732,25 +804,25 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
         <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
       </c>
       <c r="L5">
         <v>15</v>
@@ -758,7 +830,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -770,25 +842,25 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
         <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
-        <v>22</v>
       </c>
       <c r="L6">
         <v>15</v>
@@ -796,7 +868,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -808,25 +880,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
         <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
       </c>
       <c r="L7">
         <v>15</v>
@@ -834,7 +906,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -846,25 +918,25 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
         <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
       </c>
       <c r="L8">
         <v>15</v>
@@ -872,7 +944,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -884,16 +956,16 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
+      <c r="G9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I9">
         <v>8</v>
@@ -902,7 +974,7 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L9">
         <v>15</v>
@@ -910,7 +982,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -922,16 +994,16 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I10">
         <v>8</v>
@@ -940,7 +1012,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L10">
         <v>15</v>
@@ -948,7 +1020,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -960,25 +1032,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
         <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
-      </c>
-      <c r="J11">
-        <v>8</v>
-      </c>
-      <c r="K11" t="s">
-        <v>22</v>
       </c>
       <c r="L11">
         <v>15</v>
@@ -986,7 +1058,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -998,25 +1070,25 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
         <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12">
-        <v>8</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12" t="s">
-        <v>22</v>
       </c>
       <c r="L12">
         <v>5</v>
@@ -1024,7 +1096,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1036,25 +1108,25 @@
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
         <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
-      </c>
-      <c r="J13">
-        <v>4</v>
-      </c>
-      <c r="K13" t="s">
-        <v>22</v>
       </c>
       <c r="L13">
         <v>10</v>
@@ -1062,37 +1134,37 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
         <v>20</v>
-      </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14">
-        <v>8</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
-      </c>
-      <c r="K14" t="s">
-        <v>22</v>
       </c>
       <c r="L14">
         <v>20</v>
@@ -1100,7 +1172,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1117,11 +1189,11 @@
       <c r="F15" t="s">
         <v>19</v>
       </c>
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>21</v>
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I15">
         <v>8</v>
@@ -1130,7 +1202,7 @@
         <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L15">
         <v>15</v>
@@ -1141,7 +1213,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1158,11 +1230,11 @@
       <c r="F16" t="s">
         <v>19</v>
       </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" t="s">
-        <v>21</v>
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I16">
         <v>8</v>
@@ -1171,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L16">
         <v>15</v>
@@ -1185,7 +1257,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -1202,11 +1274,11 @@
       <c r="F17" t="s">
         <v>19</v>
       </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
+      <c r="G17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I17">
         <v>8</v>
@@ -1215,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="L17">
         <v>15</v>
@@ -1223,7 +1295,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -1240,11 +1312,11 @@
       <c r="F18" t="s">
         <v>19</v>
       </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>21</v>
+      <c r="G18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I18">
         <v>8</v>
@@ -1253,7 +1325,7 @@
         <v>4</v>
       </c>
       <c r="K18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L18">
         <v>15</v>

</xml_diff>